<commit_message>
added requirments, modified readme, added timer to input, added database
</commit_message>
<xml_diff>
--- a/productTable.xlsx
+++ b/productTable.xlsx
@@ -536,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="n">
-        <v>2.23</v>
+        <v>2.24</v>
       </c>
       <c r="J2" t="n">
         <v>2.12</v>
@@ -592,7 +592,7 @@
         <v>247</v>
       </c>
       <c r="I3" t="n">
-        <v>55.03</v>
+        <v>55.31</v>
       </c>
       <c r="J3" t="n">
         <v>52.45</v>
@@ -648,7 +648,7 @@
         <v>67</v>
       </c>
       <c r="I4" t="n">
-        <v>14.93</v>
+        <v>15</v>
       </c>
       <c r="J4" t="n">
         <v>14.23</v>
@@ -704,7 +704,7 @@
         <v>30</v>
       </c>
       <c r="I5" t="n">
-        <v>6.68</v>
+        <v>6.72</v>
       </c>
       <c r="J5" t="n">
         <v>6.37</v>
@@ -760,10 +760,10 @@
         <v>538</v>
       </c>
       <c r="I6" t="n">
-        <v>119.87</v>
+        <v>120.48</v>
       </c>
       <c r="J6" t="n">
-        <v>114.23</v>
+        <v>114.24</v>
       </c>
       <c r="K6" t="n">
         <v>83766</v>
@@ -816,7 +816,7 @@
         <v>140</v>
       </c>
       <c r="I7" t="n">
-        <v>31.19</v>
+        <v>31.35</v>
       </c>
       <c r="J7" t="n">
         <v>29.73</v>
@@ -872,7 +872,7 @@
         <v>270</v>
       </c>
       <c r="I8" t="n">
-        <v>60.16</v>
+        <v>60.46</v>
       </c>
       <c r="J8" t="n">
         <v>57.33</v>

</xml_diff>